<commit_message>
Fix cardinality issue on correlatedDiagnoses
</commit_message>
<xml_diff>
--- a/image/clinicalprofile.xlsx
+++ b/image/clinicalprofile.xlsx
@@ -8360,7 +8360,7 @@
         <v>40</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>39</v>
@@ -8435,7 +8435,7 @@
         <v>40</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>39</v>

</xml_diff>